<commit_message>
kids playing crap in the alley; can put variables into dialogue csv; dialogue condition checks
</commit_message>
<xml_diff>
--- a/assets/list of assets.xlsx
+++ b/assets/list of assets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roosevelt\Documents\GameMakerStudio2\diver-man\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DC7CB9-89F9-4DE0-B5A5-16E335E97F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8437F6-3AE5-413E-BEE1-A36F4F8505A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
   <si>
     <t>characters</t>
   </si>
@@ -129,9 +129,6 @@
     <t>brother playing flute</t>
   </si>
   <si>
-    <t>bag of gold</t>
-  </si>
-  <si>
     <t>diverman opening chest</t>
   </si>
   <si>
@@ -181,6 +178,63 @@
   </si>
   <si>
     <t>crab knocked</t>
+  </si>
+  <si>
+    <t>gui</t>
+  </si>
+  <si>
+    <t>boxes</t>
+  </si>
+  <si>
+    <t>coins</t>
+  </si>
+  <si>
+    <t>hermit crab</t>
+  </si>
+  <si>
+    <t>textbox paper</t>
+  </si>
+  <si>
+    <t>textbox bubbles</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>sandwich</t>
+  </si>
+  <si>
+    <t>vendors daughter</t>
+  </si>
+  <si>
+    <t>vendor stand</t>
+  </si>
+  <si>
+    <t>fence</t>
+  </si>
+  <si>
+    <t>lightpole</t>
+  </si>
+  <si>
+    <t>truck</t>
+  </si>
+  <si>
+    <t>fountain</t>
+  </si>
+  <si>
+    <t>sailor pete sleeping and sitting</t>
+  </si>
+  <si>
+    <t>sailor pete 'scare' animation</t>
+  </si>
+  <si>
+    <t>brother wedgied on the dock pole</t>
+  </si>
+  <si>
+    <t>seagull</t>
+  </si>
+  <si>
+    <t>seagull flying</t>
   </si>
 </sst>
 </file>
@@ -210,7 +264,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +289,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -248,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -257,6 +323,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,262 +614,360 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="K2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="K5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="9"/>
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K7" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="E8" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B9" s="9"/>
+      <c r="E9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="E10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="E11" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="B12" s="9"/>
+      <c r="E12" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="E13" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="E14" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="E15" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+      <c r="E16" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="E17" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="E18" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="9"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="9"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D13" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="9"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="9"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="B34" s="9"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B35" s="9"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="B36" s="9"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bugfix - dialogue with a variable not lining up
</commit_message>
<xml_diff>
--- a/assets/list of assets.xlsx
+++ b/assets/list of assets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roosevelt\Documents\GameMakerStudio2\diver-man\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EBFCF9-ABE3-4A7D-B46D-CFDE14E694B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338E6A62-5366-41E5-8A8E-9E68D8EC09C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
   <si>
     <t>characters</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>chef mafioso with head out window</t>
+  </si>
+  <si>
+    <t>street garbage</t>
   </si>
 </sst>
 </file>
@@ -660,7 +663,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +981,9 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
-      <c r="E24" s="9"/>
+      <c r="E24" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">

</xml_diff>

<commit_message>
draw_shadow_ext() is back in
</commit_message>
<xml_diff>
--- a/assets/list of assets.xlsx
+++ b/assets/list of assets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roosevelt\Documents\GameMakerStudio2\diver-man\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338E6A62-5366-41E5-8A8E-9E68D8EC09C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF805C1-46AB-402D-8D2B-F2E03AEB2B38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -663,7 +663,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +825,7 @@
       <c r="C8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -986,7 +986,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B25" s="9"/>

</xml_diff>

<commit_message>
got in a lot
</commit_message>
<xml_diff>
--- a/assets/list of assets.xlsx
+++ b/assets/list of assets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roosevelt\Documents\GameMakerStudio2\diver-man\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF805C1-46AB-402D-8D2B-F2E03AEB2B38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BCC27D-F8A9-4829-9259-C8EA74103463}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="86">
   <si>
     <t>characters</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>street garbage</t>
+  </si>
+  <si>
+    <t>bobs rooftop garden</t>
   </si>
 </sst>
 </file>
@@ -663,7 +666,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,6 +876,9 @@
         <v>5</v>
       </c>
       <c r="B12" s="9"/>
+      <c r="C12" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="E12" s="3" t="s">
         <v>60</v>
       </c>
@@ -881,7 +887,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="9"/>
@@ -1022,7 +1028,7 @@
       <c r="B32" s="9"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="6" t="s">
         <v>73</v>
       </c>
       <c r="B33" s="9"/>

</xml_diff>

<commit_message>
fixed intro text crash
</commit_message>
<xml_diff>
--- a/assets/list of assets.xlsx
+++ b/assets/list of assets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roosevelt\Documents\GameMakerStudio2\diver-man\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roose\Documents\GameMakerStudio2\diver-man\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BCC27D-F8A9-4829-9259-C8EA74103463}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941BD313-A03B-4DC6-99C2-23C46E36F5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -666,7 +666,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +882,7 @@
       <c r="E12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="4" t="s">
         <v>83</v>
       </c>
     </row>
@@ -894,7 +894,7 @@
       <c r="E13" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -906,7 +906,7 @@
       <c r="E14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="K14" s="4" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>